<commit_message>
Add some total minute OnCallData
</commit_message>
<xml_diff>
--- a/src/main/resources/call.xlsx
+++ b/src/main/resources/call.xlsx
@@ -11,35 +11,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Desenvolvedor</t>
   </si>
   <si>
-    <t xml:space="preserve">Total time </t>
+    <t xml:space="preserve">Inicio </t>
   </si>
   <si>
-    <t>Total value</t>
+    <t>fim</t>
   </si>
   <si>
     <t>Matheus</t>
   </si>
   <si>
+    <t>18:00:00</t>
+  </si>
+  <si>
+    <t>22:30:00</t>
+  </si>
+  <si>
     <t>Thiago</t>
   </si>
   <si>
+    <t>05:00:00</t>
+  </si>
+  <si>
+    <t>10:50:00</t>
+  </si>
+  <si>
+    <t>16:40:00</t>
+  </si>
+  <si>
     <t>Jonas</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>08:00:00</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>13:45:00</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>07:00:00</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -62,8 +97,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <color indexed="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -93,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -137,6 +177,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="12"/>
       </left>
@@ -152,13 +203,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -169,22 +260,46 @@
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="59" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="59" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,12 +521,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -444,10 +559,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -695,12 +810,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1015,10 +1130,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1272,13 +1387,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.0391" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="3" width="12.6719" style="1" customWidth="1"/>
     <col min="4" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
@@ -1294,37 +1409,2160 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="13.65" customHeight="1">
+    <row r="2" ht="19.55" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="C2" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
+      <c r="B2" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="19.55" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1.208333333333333</v>
-      </c>
-      <c r="C3" s="8">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="19.55" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1.694444444444444</v>
-      </c>
-      <c r="C4" s="8">
-        <v>5000</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" ht="19.55" customHeight="1">
+      <c r="A5" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" ht="19.55" customHeight="1">
+      <c r="A6" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" ht="19.55" customHeight="1">
+      <c r="A7" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" ht="19.55" customHeight="1">
+      <c r="A8" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" ht="19.55" customHeight="1">
+      <c r="A9" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" ht="19.55" customHeight="1">
+      <c r="A10" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" ht="19.55" customHeight="1">
+      <c r="A11" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" ht="19.55" customHeight="1">
+      <c r="A12" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" ht="19.55" customHeight="1">
+      <c r="A13" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" ht="19.55" customHeight="1">
+      <c r="A14" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" ht="19.55" customHeight="1">
+      <c r="A15" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" ht="19.55" customHeight="1">
+      <c r="A16" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" ht="19.55" customHeight="1">
+      <c r="A17" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" ht="19.55" customHeight="1">
+      <c r="A18" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" ht="19.55" customHeight="1">
+      <c r="A19" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" ht="19.55" customHeight="1">
+      <c r="A20" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" ht="19.55" customHeight="1">
+      <c r="A21" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" ht="19.55" customHeight="1">
+      <c r="A22" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" ht="19.55" customHeight="1">
+      <c r="A23" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" ht="19.55" customHeight="1">
+      <c r="A24" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" ht="19.55" customHeight="1">
+      <c r="A25" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" ht="19.55" customHeight="1">
+      <c r="A26" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" ht="19.55" customHeight="1">
+      <c r="A27" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" ht="19.55" customHeight="1">
+      <c r="A28" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" ht="19.55" customHeight="1">
+      <c r="A29" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" ht="19.55" customHeight="1">
+      <c r="A30" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" ht="19.55" customHeight="1">
+      <c r="A31" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" ht="19.55" customHeight="1">
+      <c r="A32" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" ht="19.55" customHeight="1">
+      <c r="A33" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" ht="19.55" customHeight="1">
+      <c r="A34" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" ht="19.55" customHeight="1">
+      <c r="A35" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" ht="19.55" customHeight="1">
+      <c r="A36" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" ht="19.55" customHeight="1">
+      <c r="A37" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" ht="19.55" customHeight="1">
+      <c r="A38" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" ht="19.55" customHeight="1">
+      <c r="A39" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" ht="19.55" customHeight="1">
+      <c r="A40" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" ht="19.55" customHeight="1">
+      <c r="A41" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" ht="19.55" customHeight="1">
+      <c r="A42" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" ht="19.55" customHeight="1">
+      <c r="A43" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" ht="19.55" customHeight="1">
+      <c r="A44" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" ht="19.55" customHeight="1">
+      <c r="A45" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" ht="19.55" customHeight="1">
+      <c r="A46" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" ht="19.55" customHeight="1">
+      <c r="A47" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" ht="19.55" customHeight="1">
+      <c r="A48" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" ht="19.55" customHeight="1">
+      <c r="A49" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" ht="19.55" customHeight="1">
+      <c r="A50" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" ht="19.55" customHeight="1">
+      <c r="A51" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" ht="19.55" customHeight="1">
+      <c r="A52" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" ht="19.55" customHeight="1">
+      <c r="A53" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" ht="19.55" customHeight="1">
+      <c r="A54" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" ht="19.55" customHeight="1">
+      <c r="A55" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" ht="19.55" customHeight="1">
+      <c r="A56" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" ht="19.55" customHeight="1">
+      <c r="A57" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" ht="19.55" customHeight="1">
+      <c r="A58" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" ht="19.55" customHeight="1">
+      <c r="A59" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" ht="19.55" customHeight="1">
+      <c r="A60" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" ht="19.55" customHeight="1">
+      <c r="A61" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C61" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" ht="19.55" customHeight="1">
+      <c r="A62" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" ht="19.55" customHeight="1">
+      <c r="A63" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B63" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" ht="19.55" customHeight="1">
+      <c r="A64" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" ht="19.55" customHeight="1">
+      <c r="A65" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" ht="19.55" customHeight="1">
+      <c r="A66" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B66" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" ht="19.55" customHeight="1">
+      <c r="A67" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" ht="19.55" customHeight="1">
+      <c r="A68" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C68" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" ht="19.55" customHeight="1">
+      <c r="A69" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" ht="19.55" customHeight="1">
+      <c r="A70" t="s" s="12">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" ht="19.55" customHeight="1">
+      <c r="A71" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" ht="19.55" customHeight="1">
+      <c r="A72" t="s" s="12">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" ht="19.55" customHeight="1">
+      <c r="A73" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" ht="19.55" customHeight="1">
+      <c r="A74" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" ht="19.55" customHeight="1">
+      <c r="A75" t="s" s="13">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" ht="19.55" customHeight="1">
+      <c r="A76" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" ht="19.55" customHeight="1">
+      <c r="A77" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" ht="19.55" customHeight="1">
+      <c r="A78" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B78" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C78" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" ht="19.55" customHeight="1">
+      <c r="A79" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C79" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" ht="19.55" customHeight="1">
+      <c r="A80" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B80" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C80" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" ht="19.55" customHeight="1">
+      <c r="A81" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B81" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" ht="19.55" customHeight="1">
+      <c r="A82" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C82" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" ht="19.55" customHeight="1">
+      <c r="A83" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B83" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C83" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" ht="19.55" customHeight="1">
+      <c r="A84" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C84" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" ht="19.55" customHeight="1">
+      <c r="A85" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" ht="19.55" customHeight="1">
+      <c r="A86" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C86" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" ht="19.55" customHeight="1">
+      <c r="A87" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B87" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" ht="19.55" customHeight="1">
+      <c r="A88" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" ht="19.55" customHeight="1">
+      <c r="A89" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B89" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C89" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" ht="19.55" customHeight="1">
+      <c r="A90" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B90" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" ht="19.55" customHeight="1">
+      <c r="A91" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B91" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C91" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" ht="19.55" customHeight="1">
+      <c r="A92" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B92" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C92" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" ht="19.55" customHeight="1">
+      <c r="A93" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B93" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" ht="19.55" customHeight="1">
+      <c r="A94" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" ht="19.55" customHeight="1">
+      <c r="A95" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" ht="19.55" customHeight="1">
+      <c r="A96" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C96" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" ht="19.55" customHeight="1">
+      <c r="A97" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B97" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C97" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" ht="19.55" customHeight="1">
+      <c r="A98" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B98" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C98" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" ht="19.55" customHeight="1">
+      <c r="A99" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B99" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C99" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" ht="19.55" customHeight="1">
+      <c r="A100" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C100" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" ht="19.55" customHeight="1">
+      <c r="A101" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B101" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C101" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" ht="19.55" customHeight="1">
+      <c r="A102" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="B102" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" ht="19.55" customHeight="1">
+      <c r="A103" t="s" s="13">
+        <v>3</v>
+      </c>
+      <c r="B103" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C103" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" ht="19.55" customHeight="1">
+      <c r="A104" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B104" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C104" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" ht="19.55" customHeight="1">
+      <c r="A105" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B105" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" ht="19.55" customHeight="1">
+      <c r="A106" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B106" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C106" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" ht="19.55" customHeight="1">
+      <c r="A107" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B107" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C107" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" ht="19.55" customHeight="1">
+      <c r="A108" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B108" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C108" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" ht="19.55" customHeight="1">
+      <c r="A109" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B109" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" ht="19.55" customHeight="1">
+      <c r="A110" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B110" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C110" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" ht="19.55" customHeight="1">
+      <c r="A111" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B111" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C111" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" ht="19.55" customHeight="1">
+      <c r="A112" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B112" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C112" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" ht="19.55" customHeight="1">
+      <c r="A113" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B113" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C113" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" ht="19.55" customHeight="1">
+      <c r="A114" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B114" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C114" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" ht="19.55" customHeight="1">
+      <c r="A115" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B115" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" ht="19.55" customHeight="1">
+      <c r="A116" t="s" s="13">
+        <v>3</v>
+      </c>
+      <c r="B116" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C116" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" ht="19.55" customHeight="1">
+      <c r="A117" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B117" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C117" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" ht="19.55" customHeight="1">
+      <c r="A118" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B118" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C118" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" ht="19.55" customHeight="1">
+      <c r="A119" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B119" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C119" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" ht="19.55" customHeight="1">
+      <c r="A120" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B120" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C120" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" ht="19.55" customHeight="1">
+      <c r="A121" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B121" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C121" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" ht="19.55" customHeight="1">
+      <c r="A122" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B122" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" ht="19.55" customHeight="1">
+      <c r="A123" t="s" s="13">
+        <v>3</v>
+      </c>
+      <c r="B123" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C123" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" ht="19.55" customHeight="1">
+      <c r="A124" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B124" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C124" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" ht="19.55" customHeight="1">
+      <c r="A125" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B125" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C125" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" ht="19.55" customHeight="1">
+      <c r="A126" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B126" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C126" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" ht="19.55" customHeight="1">
+      <c r="A127" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B127" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C127" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" ht="19.55" customHeight="1">
+      <c r="A128" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B128" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C128" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" ht="19.55" customHeight="1">
+      <c r="A129" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="B129" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" ht="19.55" customHeight="1">
+      <c r="A130" t="s" s="13">
+        <v>3</v>
+      </c>
+      <c r="B130" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C130" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" ht="19.55" customHeight="1">
+      <c r="A131" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B131" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C131" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" ht="19.55" customHeight="1">
+      <c r="A132" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B132" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C132" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" ht="19.55" customHeight="1">
+      <c r="A133" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B133" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C133" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" ht="19.55" customHeight="1">
+      <c r="A134" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B134" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C134" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" ht="19.55" customHeight="1">
+      <c r="A135" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B135" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C135" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" ht="19.55" customHeight="1">
+      <c r="A136" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B136" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C136" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" ht="19.55" customHeight="1">
+      <c r="A137" t="s" s="13">
+        <v>3</v>
+      </c>
+      <c r="B137" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C137" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" ht="19.55" customHeight="1">
+      <c r="A138" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B138" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C138" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" ht="19.55" customHeight="1">
+      <c r="A139" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B139" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C139" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" ht="19.55" customHeight="1">
+      <c r="A140" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B140" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C140" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" ht="19.55" customHeight="1">
+      <c r="A141" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B141" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C141" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" ht="19.55" customHeight="1">
+      <c r="A142" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B142" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C142" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" ht="19.55" customHeight="1">
+      <c r="A143" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B143" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C143" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" ht="19.55" customHeight="1">
+      <c r="A144" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B144" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C144" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" ht="19.55" customHeight="1">
+      <c r="A145" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B145" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C145" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" ht="19.55" customHeight="1">
+      <c r="A146" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B146" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C146" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" ht="19.55" customHeight="1">
+      <c r="A147" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B147" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C147" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" ht="19.55" customHeight="1">
+      <c r="A148" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B148" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C148" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" ht="19.55" customHeight="1">
+      <c r="A149" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B149" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C149" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" ht="19.55" customHeight="1">
+      <c r="A150" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B150" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C150" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" ht="19.55" customHeight="1">
+      <c r="A151" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B151" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C151" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" ht="19.55" customHeight="1">
+      <c r="A152" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B152" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C152" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" ht="19.55" customHeight="1">
+      <c r="A153" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B153" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C153" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" ht="19.55" customHeight="1">
+      <c r="A154" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B154" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C154" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" ht="19.55" customHeight="1">
+      <c r="A155" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B155" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C155" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" ht="19.55" customHeight="1">
+      <c r="A156" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="B156" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C156" t="s" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="157" ht="19.55" customHeight="1">
+      <c r="A157" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B157" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="C157" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" ht="19.55" customHeight="1">
+      <c r="A158" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B158" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C158" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" ht="19.55" customHeight="1">
+      <c r="A159" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B159" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C159" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" ht="19.55" customHeight="1">
+      <c r="A160" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B160" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C160" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" ht="19.55" customHeight="1">
+      <c r="A161" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B161" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C161" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" ht="19.55" customHeight="1">
+      <c r="A162" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C162" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" ht="19.55" customHeight="1">
+      <c r="A163" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B163" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C163" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" ht="19.55" customHeight="1">
+      <c r="A164" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="B164" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C164" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" ht="19.55" customHeight="1">
+      <c r="A165" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B165" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C165" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" ht="19.55" customHeight="1">
+      <c r="A166" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B166" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C166" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" ht="19.55" customHeight="1">
+      <c r="A167" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B167" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C167" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" ht="19.55" customHeight="1">
+      <c r="A168" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B168" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C168" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" ht="19.55" customHeight="1">
+      <c r="A169" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B169" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C169" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170" ht="19.55" customHeight="1">
+      <c r="A170" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B170" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C170" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" ht="19.55" customHeight="1">
+      <c r="A171" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B171" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C171" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" ht="19.55" customHeight="1">
+      <c r="A172" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B172" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C172" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" ht="19.55" customHeight="1">
+      <c r="A173" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B173" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C173" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" ht="19.55" customHeight="1">
+      <c r="A174" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B174" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C174" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" ht="19.55" customHeight="1">
+      <c r="A175" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B175" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C175" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" ht="19.55" customHeight="1">
+      <c r="A176" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B176" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C176" t="s" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="177" ht="19.55" customHeight="1">
+      <c r="A177" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B177" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="C177" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="178" ht="19.55" customHeight="1">
+      <c r="A178" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B178" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C178" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" ht="19.55" customHeight="1">
+      <c r="A179" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B179" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C179" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" ht="19.55" customHeight="1">
+      <c r="A180" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B180" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C180" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" ht="19.55" customHeight="1">
+      <c r="A181" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B181" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C181" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" ht="19.55" customHeight="1">
+      <c r="A182" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B182" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C182" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="183" ht="19.55" customHeight="1">
+      <c r="A183" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B183" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C183" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" ht="19.55" customHeight="1">
+      <c r="A184" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B184" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C184" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" ht="19.55" customHeight="1">
+      <c r="A185" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B185" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C185" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" ht="19.55" customHeight="1">
+      <c r="A186" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B186" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C186" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" ht="19.55" customHeight="1">
+      <c r="A187" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B187" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C187" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" ht="19.55" customHeight="1">
+      <c r="A188" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B188" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C188" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" ht="19.55" customHeight="1">
+      <c r="A189" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B189" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C189" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="190" ht="19.55" customHeight="1">
+      <c r="A190" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B190" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C190" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" ht="19.55" customHeight="1">
+      <c r="A191" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B191" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C191" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" ht="19.55" customHeight="1">
+      <c r="A192" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B192" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C192" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" ht="19.55" customHeight="1">
+      <c r="A193" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B193" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C193" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" ht="19.55" customHeight="1">
+      <c r="A194" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B194" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C194" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" ht="19.55" customHeight="1">
+      <c r="A195" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B195" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C195" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" ht="19.55" customHeight="1">
+      <c r="A196" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B196" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C196" t="s" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="197" ht="19.55" customHeight="1">
+      <c r="A197" t="s" s="14">
+        <v>3</v>
+      </c>
+      <c r="B197" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="C197" t="s" s="16">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add colunm value 33% + Clean Code
</commit_message>
<xml_diff>
--- a/src/main/resources/call.xlsx
+++ b/src/main/resources/call.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Desenvolvedor</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>17:00:00</t>
+  </si>
+  <si>
+    <t>Ana</t>
   </si>
 </sst>
 </file>
@@ -292,13 +295,13 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1387,7 +1390,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3555,14 +3558,80 @@
       </c>
     </row>
     <row r="197" ht="19.55" customHeight="1">
-      <c r="A197" t="s" s="14">
-        <v>3</v>
-      </c>
-      <c r="B197" t="s" s="15">
+      <c r="A197" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B197" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="C197" t="s" s="16">
+      <c r="C197" t="s" s="8">
         <v>17</v>
+      </c>
+    </row>
+    <row r="198" ht="19.55" customHeight="1">
+      <c r="A198" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="B198" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="C198" t="s" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" ht="19.55" customHeight="1">
+      <c r="A199" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="B199" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C199" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" ht="19.55" customHeight="1">
+      <c r="A200" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B200" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C200" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" ht="19.55" customHeight="1">
+      <c r="A201" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B201" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C201" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" ht="19.55" customHeight="1">
+      <c r="A202" t="s" s="9">
+        <v>3</v>
+      </c>
+      <c r="B202" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C202" t="s" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" ht="19.55" customHeight="1">
+      <c r="A203" t="s" s="14">
+        <v>6</v>
+      </c>
+      <c r="B203" t="s" s="15">
+        <v>4</v>
+      </c>
+      <c r="C203" t="s" s="16">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>